<commit_message>
Cash service update, interest increase assumption removed removed
Fix #29
</commit_message>
<xml_diff>
--- a/NNB data.xlsx
+++ b/NNB data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="420" windowWidth="28800" windowHeight="13275" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="420" windowWidth="28800" windowHeight="13275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="total nnb" sheetId="1" r:id="rId1"/>
@@ -401,8 +401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F865"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="G131" sqref="G131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,15 +1503,24 @@
       <c r="A134" s="1">
         <v>42947</v>
       </c>
+      <c r="B134" s="2">
+        <v>513333333.33333331</v>
+      </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>42978</v>
       </c>
+      <c r="B135" s="2">
+        <v>513333333.33333331</v>
+      </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>43007</v>
+      </c>
+      <c r="B136" s="2">
+        <v>513333333.33333331</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
@@ -4256,8 +4265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEFEAE08-7DFF-4A8E-8EBA-42D957E8AC02}">
   <dimension ref="A1:B409"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="F126" sqref="F126"/>
+    <sheetView topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="B136" sqref="B136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Oct-fair value update, reflect interest rate increase
fix #32
</commit_message>
<xml_diff>
--- a/NNB data.xlsx
+++ b/NNB data.xlsx
@@ -402,7 +402,7 @@
   <dimension ref="A1:F865"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="G131" sqref="G131"/>
+      <selection activeCell="F135" sqref="F135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1504,7 +1504,7 @@
         <v>42947</v>
       </c>
       <c r="B134" s="2">
-        <v>513333333.33333331</v>
+        <v>513333333.33333302</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
@@ -1512,7 +1512,7 @@
         <v>42978</v>
       </c>
       <c r="B135" s="2">
-        <v>513333333.33333331</v>
+        <v>513333333.33333302</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
@@ -1520,7 +1520,7 @@
         <v>43007</v>
       </c>
       <c r="B136" s="2">
-        <v>513333333.33333331</v>
+        <v>513333333.33333302</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
20-04-2018 funds data update
</commit_message>
<xml_diff>
--- a/NNB data.xlsx
+++ b/NNB data.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cl\Documents\HL_model_git\HL\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8959390-18D6-49CA-A075-2A9619C7466F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="840" windowWidth="28800" windowHeight="13275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1680" windowWidth="28800" windowHeight="13275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="total nnb" sheetId="1" r:id="rId1"/>
     <sheet name="clients" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,12 +26,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>NNB</t>
   </si>
   <si>
-    <t>client number</t>
+    <t>Net new clients</t>
+  </si>
+  <si>
+    <t>No. of clients</t>
   </si>
 </sst>
 </file>
@@ -64,7 +68,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -72,18 +76,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -399,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F865"/>
+  <dimension ref="A1:N865"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="E134" sqref="E134"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="E115" sqref="E115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,12 +435,12 @@
     <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>38929</v>
       </c>
@@ -428,15 +448,19 @@
         <v>175000000.00000003</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>38960</v>
       </c>
       <c r="B3" s="2">
         <v>175000000.00000003</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>38989</v>
       </c>
@@ -444,7 +468,7 @@
         <v>175000000.00000003</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>39021</v>
       </c>
@@ -452,7 +476,7 @@
         <v>175000000.00000003</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>39051</v>
       </c>
@@ -460,7 +484,7 @@
         <v>175000000.00000003</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>39080</v>
       </c>
@@ -468,7 +492,7 @@
         <v>175000000.00000003</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>39113</v>
       </c>
@@ -476,7 +500,7 @@
         <v>175000000.00000003</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>39141</v>
       </c>
@@ -484,7 +508,7 @@
         <v>175000000.00000003</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>39171</v>
       </c>
@@ -492,7 +516,7 @@
         <v>175000000.00000003</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>39202</v>
       </c>
@@ -500,7 +524,7 @@
         <v>175000000.00000003</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>39233</v>
       </c>
@@ -508,7 +532,7 @@
         <v>175000000.00000003</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>39262</v>
       </c>
@@ -516,7 +540,7 @@
         <v>175000000.00000003</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>39294</v>
       </c>
@@ -524,7 +548,7 @@
         <v>191666666.66666666</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>39325</v>
       </c>
@@ -532,7 +556,7 @@
         <v>191666666.66666666</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>39353</v>
       </c>
@@ -1245,11 +1269,11 @@
         <v>426666666.66666669</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="1">
+    <row r="103" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="10">
         <v>42004</v>
       </c>
-      <c r="B103" s="4">
+      <c r="B103" s="11">
         <v>426666666.66666669</v>
       </c>
     </row>
@@ -1258,7 +1282,7 @@
         <v>42034</v>
       </c>
       <c r="B104" s="4">
-        <v>916666666.66666663</v>
+        <v>412500000</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -1266,7 +1290,7 @@
         <v>42062</v>
       </c>
       <c r="B105" s="4">
-        <v>916666666.66666663</v>
+        <v>412500000</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -1274,7 +1298,7 @@
         <v>42094</v>
       </c>
       <c r="B106" s="4">
-        <v>916666666.66666663</v>
+        <v>962499999.99999988</v>
       </c>
       <c r="F106" s="2"/>
     </row>
@@ -1283,7 +1307,7 @@
         <v>42124</v>
       </c>
       <c r="B107" s="4">
-        <v>349999999.99999934</v>
+        <v>962499999.99999988</v>
       </c>
       <c r="D107" s="2"/>
       <c r="F107" s="2"/>
@@ -1293,15 +1317,15 @@
         <v>42153</v>
       </c>
       <c r="B108" s="4">
-        <v>349999999.99999934</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="1">
+        <v>550000000</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="10">
         <v>42185</v>
       </c>
-      <c r="B109" s="4">
-        <v>349999999.99999934</v>
+      <c r="B109" s="11">
+        <v>550000000</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -1333,7 +1357,7 @@
         <v>42307</v>
       </c>
       <c r="B113" s="4">
-        <v>433333333.33333331</v>
+        <v>456666666.66666669</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -1341,7 +1365,7 @@
         <v>42338</v>
       </c>
       <c r="B114" s="4">
-        <v>433333333.33333331</v>
+        <v>456666666.66666669</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -1349,7 +1373,7 @@
         <v>42369</v>
       </c>
       <c r="B115" s="4">
-        <v>433333333.33333331</v>
+        <v>456666666.66666669</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -1357,7 +1381,7 @@
         <v>42398</v>
       </c>
       <c r="B116" s="4">
-        <v>766666666.66666663</v>
+        <v>345000000</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -1365,7 +1389,7 @@
         <v>42429</v>
       </c>
       <c r="B117" s="4">
-        <v>766666666.66666663</v>
+        <v>345000000</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -1373,7 +1397,7 @@
         <v>42460</v>
       </c>
       <c r="B118" s="4">
-        <v>766666666.66666663</v>
+        <v>805000000</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -1381,7 +1405,7 @@
         <v>42489</v>
       </c>
       <c r="B119" s="4">
-        <v>303333333.33333331</v>
+        <v>805000000</v>
       </c>
       <c r="D119" s="2"/>
       <c r="F119" s="2"/>
@@ -1391,15 +1415,15 @@
         <v>42521</v>
       </c>
       <c r="B120" s="4">
-        <v>303333333.33333331</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="1">
+        <v>450000000</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="6">
         <v>42551</v>
       </c>
-      <c r="B121" s="4">
-        <v>303333333.33333331</v>
+      <c r="B121" s="9">
+        <v>450000000</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -1455,7 +1479,7 @@
         <v>42766</v>
       </c>
       <c r="B128" s="4">
-        <v>1100000000</v>
+        <v>495000000</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -1463,7 +1487,7 @@
         <v>42794</v>
       </c>
       <c r="B129" s="4">
-        <v>1100000000</v>
+        <v>495000000</v>
       </c>
       <c r="F129" s="5"/>
     </row>
@@ -1472,7 +1496,7 @@
         <v>42825</v>
       </c>
       <c r="B130" s="4">
-        <v>1100000000</v>
+        <v>1155000000</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
@@ -1480,7 +1504,7 @@
         <v>42853</v>
       </c>
       <c r="B131" s="4">
-        <v>420000000</v>
+        <v>1155000000</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
@@ -1488,7 +1512,7 @@
         <v>42886</v>
       </c>
       <c r="B132" s="4">
-        <v>420000000</v>
+        <v>650000000</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
@@ -1496,7 +1520,7 @@
         <v>42916</v>
       </c>
       <c r="B133" s="4">
-        <v>420000000</v>
+        <v>650000000</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
@@ -1528,7 +1552,7 @@
         <v>43039</v>
       </c>
       <c r="B137" s="2">
-        <v>280666666.66666669</v>
+        <v>600000000</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
@@ -1536,7 +1560,7 @@
         <v>43069</v>
       </c>
       <c r="B138" s="2">
-        <v>280666666.66666669</v>
+        <v>600000000</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
@@ -1544,7 +1568,7 @@
         <v>43098</v>
       </c>
       <c r="B139" s="2">
-        <v>280666666.66666669</v>
+        <v>600000000</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
@@ -4272,94 +4296,98 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEFEAE08-7DFF-4A8E-8EBA-42D957E8AC02}">
-  <dimension ref="A1:B409"/>
+  <dimension ref="A1:C409"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="B136" sqref="B136"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C139" sqref="A74:C139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>38929</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>38960</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>38989</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>39021</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>39051</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>39080</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>39113</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>39141</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>39171</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>39202</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>39233</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>39262</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>39294</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>39325</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>39353</v>
       </c>
@@ -4616,591 +4644,668 @@
         <v>40816</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>40847</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>40877</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>40907</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>40939</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>40968</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>40998</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>41029</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>41060</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>41089</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>41121</v>
       </c>
-      <c r="B74">
-        <v>432000</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C74">
+        <v>2333</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>41152</v>
       </c>
-      <c r="B75">
-        <v>432000</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C75">
+        <v>2333</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>41180</v>
       </c>
       <c r="B76">
         <v>432000</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C76">
+        <v>2334</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>41213</v>
       </c>
-      <c r="B77">
-        <v>446000</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C77">
+        <v>4666</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>41243</v>
       </c>
-      <c r="B78">
-        <v>446000</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C78">
+        <v>4667</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>41274</v>
       </c>
       <c r="B79">
         <v>446000</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C79">
+        <v>4667</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>41305</v>
       </c>
-      <c r="B80">
-        <v>476000</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C80">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>41333</v>
       </c>
-      <c r="B81">
-        <v>476000</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C81">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>41362</v>
       </c>
       <c r="B82">
         <v>476000</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C82">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>41394</v>
       </c>
-      <c r="B83">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C83">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>41425</v>
       </c>
-      <c r="B84">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C84">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>41453</v>
       </c>
       <c r="B85">
         <v>500000</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C85">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>41486</v>
       </c>
-      <c r="B86">
-        <v>528000</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C86">
+        <v>6666</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>41516</v>
       </c>
-      <c r="B87">
-        <v>528000</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C87">
+        <v>6667</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>41547</v>
       </c>
       <c r="B88">
         <v>528000</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C88">
+        <v>6667</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>41578</v>
       </c>
-      <c r="B89">
-        <v>584000</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C89">
+        <v>18666</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>41607</v>
       </c>
-      <c r="B90">
-        <v>584000</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C90">
+        <v>18667</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>41639</v>
       </c>
       <c r="B91">
         <v>584000</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C91">
+        <v>18667</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>41670</v>
       </c>
-      <c r="B92">
-        <v>595000</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C92">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>41698</v>
       </c>
-      <c r="B93">
-        <v>606000</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C93">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>41729</v>
       </c>
       <c r="B94">
         <v>617000</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C94">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>41759</v>
       </c>
-      <c r="B95">
-        <v>628666</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C95">
+        <v>11666</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>41789</v>
       </c>
-      <c r="B96">
-        <v>640332</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="1">
+      <c r="C96">
+        <v>11667</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="6">
         <v>41820</v>
       </c>
-      <c r="B97">
+      <c r="B97" s="7">
         <v>652000</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C97" s="7">
+        <v>11667</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>41851</v>
       </c>
-      <c r="B98">
-        <v>655333</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C98">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>41880</v>
       </c>
-      <c r="B99">
-        <v>658666</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C99">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>41912</v>
       </c>
       <c r="B100">
         <v>662000</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C100">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>41943</v>
       </c>
-      <c r="B101">
-        <v>666333</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C101">
+        <v>4667</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>41971</v>
       </c>
-      <c r="B102">
-        <v>670666</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C102">
+        <v>4666</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>42004</v>
       </c>
       <c r="B103">
         <v>675000</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C103">
+        <v>4667</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>42034</v>
       </c>
-      <c r="B104">
-        <v>688333</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C104">
+        <f>40000*0.15</f>
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>42062</v>
       </c>
-      <c r="B105">
-        <v>701666</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C105">
+        <f>40000*0.15</f>
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>42094</v>
       </c>
       <c r="B106">
         <v>715000</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C106">
+        <v>16400</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>42124</v>
       </c>
-      <c r="B107">
-        <v>722000</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C107">
+        <v>11600</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>42153</v>
       </c>
-      <c r="B108">
-        <v>729000</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C108">
+        <v>10500</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>42185</v>
       </c>
       <c r="B109">
         <v>736000</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C109">
+        <v>10500</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>42216</v>
       </c>
-      <c r="B110">
-        <v>744000</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C110">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>42247</v>
       </c>
-      <c r="B111">
-        <v>752000</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C111">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>42277</v>
       </c>
       <c r="B112">
         <v>760000</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C112">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>42307</v>
       </c>
-      <c r="B113">
-        <v>767666</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C113">
+        <v>7666</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>42338</v>
       </c>
-      <c r="B114">
-        <v>775332</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C114">
+        <v>7667</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>42369</v>
       </c>
       <c r="B115">
         <v>783000</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C115">
+        <v>7667</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>42398</v>
       </c>
-      <c r="B116">
-        <v>796000</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C116">
+        <v>5850</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>42429</v>
       </c>
-      <c r="B117">
-        <v>809000</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C117">
+        <v>5850</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>42460</v>
       </c>
       <c r="B118">
         <v>822000</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C118">
+        <v>15400</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>42489</v>
       </c>
-      <c r="B119">
-        <v>826666</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C119">
+        <v>11900</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>42521</v>
       </c>
-      <c r="B120">
-        <v>831332</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C120">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>42551</v>
       </c>
       <c r="B121">
         <v>836000</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C121">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>42580</v>
       </c>
-      <c r="B122">
-        <v>842666</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C122">
+        <v>6666</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>42613</v>
       </c>
-      <c r="B123">
-        <v>849332</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C123">
+        <v>6667</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>42643</v>
       </c>
       <c r="B124">
         <v>856000</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C124">
+        <v>6667</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>42674</v>
       </c>
-      <c r="B125">
-        <v>862666</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C125">
+        <v>6666</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>42704</v>
       </c>
-      <c r="B126">
-        <v>869332</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C126">
+        <v>6667</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>42734</v>
       </c>
       <c r="B127">
         <v>876000</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C127">
+        <v>6667</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>42766</v>
       </c>
-      <c r="B128">
-        <v>894666</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C128">
+        <v>8400</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>42794</v>
       </c>
-      <c r="B129">
-        <v>913332</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C129">
+        <v>8400</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>42825</v>
       </c>
       <c r="B130">
         <v>932000</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C130">
+        <v>19600</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>42853</v>
       </c>
-      <c r="B131">
-        <v>939333</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C131">
+        <v>19600</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>42886</v>
       </c>
-      <c r="B132">
-        <v>946666</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C132">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>42916</v>
       </c>
       <c r="B133">
         <v>954000</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C133">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>42947</v>
       </c>
-      <c r="B134">
-        <v>965281</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C134">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>42978</v>
       </c>
-      <c r="B135">
-        <v>976562</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C135">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>43007</v>
       </c>
       <c r="B136">
-        <v>987844</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+        <v>983000</v>
+      </c>
+      <c r="C136">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>43039</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C137">
+        <v>10333</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>43069</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C138">
+        <v>10334</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>43098</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B139">
+        <v>1015000</v>
+      </c>
+      <c r="C139">
+        <v>10333</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>43131</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>43159</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>43189</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>43220</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>43251</v>
       </c>

</xml_diff>

<commit_message>
Post FY18 result update
Fix #129
Fix #130
Fix #131
</commit_message>
<xml_diff>
--- a/NNB data.xlsx
+++ b/NNB data.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cl\Documents\HL_model_git\HL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cl\Documents\HL_model_git\HL_live\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8959390-18D6-49CA-A075-2A9619C7466F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA38C751-5EE3-427B-AF04-48B4F7BCAF02}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1680" windowWidth="28800" windowHeight="13275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1680" windowWidth="28800" windowHeight="13275" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="total nnb" sheetId="1" r:id="rId1"/>
     <sheet name="clients" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -421,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N865"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="E115" sqref="E115"/>
+    <sheetView topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="H135" sqref="H135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1575,103 +1575,121 @@
       <c r="A140" s="1">
         <v>43131</v>
       </c>
+      <c r="B140" s="2">
+        <v>495000000</v>
+      </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>43159</v>
       </c>
+      <c r="B141" s="2">
+        <v>495000000</v>
+      </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>43189</v>
       </c>
+      <c r="B142" s="2">
+        <v>1155000000</v>
+      </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>43220</v>
       </c>
+      <c r="B143" s="2">
+        <v>1155000000</v>
+      </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>43251</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B144" s="2">
+        <v>480000000</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>43280</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B145" s="2">
+        <v>480000000</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>43312</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>43343</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>43371</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>43404</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>43434</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>43465</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>43496</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>43524</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>43553</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>43585</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>43616</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>43644</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>43677</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>43707</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>43738</v>
       </c>
@@ -4298,8 +4316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEFEAE08-7DFF-4A8E-8EBA-42D957E8AC02}">
   <dimension ref="A1:C409"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C139" sqref="A74:C139"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="E136" sqref="E136:E146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5289,103 +5307,127 @@
       <c r="A140" s="1">
         <v>43131</v>
       </c>
+      <c r="C140">
+        <v>10650</v>
+      </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>43159</v>
       </c>
+      <c r="C141">
+        <v>10650</v>
+      </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>43189</v>
       </c>
+      <c r="B142">
+        <v>1057600</v>
+      </c>
+      <c r="C142">
+        <v>21300</v>
+      </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>43220</v>
       </c>
+      <c r="C143">
+        <v>16700</v>
+      </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>43251</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C144">
+        <v>8350</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>43280</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B145">
+        <v>1091000</v>
+      </c>
+      <c r="C145">
+        <v>8350</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>43312</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>43343</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>43371</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>43404</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>43434</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>43465</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>43496</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>43524</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>43553</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>43585</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>43616</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>43644</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>43677</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>43707</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>43738</v>
       </c>

</xml_diff>

<commit_message>
Dec 2018 end update
</commit_message>
<xml_diff>
--- a/NNB data.xlsx
+++ b/NNB data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cl\Documents\HL_model_git\HL_live\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cl.WAVEPOWER\PycharmProjects\HL_live\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDE3DD0-2830-4EAD-8B77-225ACF1D41B8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{84DD1F94-8984-4954-BB06-7D2E47746FEB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1680" windowWidth="28800" windowHeight="13275" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,15 +16,10 @@
     <sheet name="total nnb" sheetId="1" r:id="rId1"/>
     <sheet name="clients" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021" concurrentCalc="0"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -427,7 +422,7 @@
   <dimension ref="A1:N865"/>
   <sheetViews>
     <sheetView topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="H135" sqref="H135"/>
+      <selection activeCell="F141" sqref="F141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1628,15 +1623,24 @@
       <c r="A146" s="1">
         <v>43312</v>
       </c>
+      <c r="B146" s="2">
+        <v>433333333.33333331</v>
+      </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>43343</v>
       </c>
+      <c r="B147" s="2">
+        <v>433333333.33333331</v>
+      </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>43371</v>
+      </c>
+      <c r="B148" s="2">
+        <v>433333333.33333331</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
@@ -4321,8 +4325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEFEAE08-7DFF-4A8E-8EBA-42D957E8AC02}">
   <dimension ref="A1:E409"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="G124" sqref="G124"/>
+    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
+      <selection activeCell="L144" sqref="L144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5366,15 +5370,27 @@
       <c r="A146" s="1">
         <v>43312</v>
       </c>
+      <c r="C146">
+        <v>9666</v>
+      </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>43343</v>
       </c>
+      <c r="C147">
+        <v>9667</v>
+      </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>43371</v>
+      </c>
+      <c r="B148">
+        <v>1120000</v>
+      </c>
+      <c r="C148">
+        <v>9667</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>